<commit_message>
added additional problem descriptions and solutions
</commit_message>
<xml_diff>
--- a/RQ1/RQ1.xlsx
+++ b/RQ1/RQ1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Documents\MastersDegree\CSI5370-SoftwareVerificationAndTesting\GithubRepos\csi5370project\RQ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310AF53A-DF7A-4DEF-B3C7-C5187A6F8CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB46A9-6285-4DD6-A18C-B9205CDB6CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,20 +200,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -498,146 +498,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -751,7 +751,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -772,6 +772,258 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
+    <row r="7" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="F2:K2"/>

</xml_diff>

<commit_message>
added 50 problems and solutions
</commit_message>
<xml_diff>
--- a/RQ1/RQ1.xlsx
+++ b/RQ1/RQ1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Documents\MastersDegree\CSI5370-SoftwareVerificationAndTesting\GithubRepos\csi5370project\RQ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2344B63C-AF6C-4A6D-99E0-9C1EA6F7F5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F899DF-6D25-4AFF-A39C-6FB31A6C1944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57705" yWindow="-2535" windowWidth="30300" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="510" windowWidth="29010" windowHeight="15075" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Data" sheetId="1" r:id="rId1"/>
+    <sheet name="ChatGPT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>SN</t>
   </si>
@@ -229,6 +230,63 @@
   </si>
   <si>
     <t>Math, String, Dynamic Programming, Recursion, Memoization</t>
+  </si>
+  <si>
+    <t>Problem27</t>
+  </si>
+  <si>
+    <t>Problem28</t>
+  </si>
+  <si>
+    <t>Problem29</t>
+  </si>
+  <si>
+    <t>Problem30</t>
+  </si>
+  <si>
+    <t>Problem31</t>
+  </si>
+  <si>
+    <t>Problem32</t>
+  </si>
+  <si>
+    <t>Problem33</t>
+  </si>
+  <si>
+    <t>Problem34</t>
+  </si>
+  <si>
+    <t>Problem35</t>
+  </si>
+  <si>
+    <t>Problem36</t>
+  </si>
+  <si>
+    <t>Problem37</t>
+  </si>
+  <si>
+    <t>Problem38</t>
+  </si>
+  <si>
+    <t>Problem39</t>
+  </si>
+  <si>
+    <t>Problem40</t>
+  </si>
+  <si>
+    <t>Problem Name</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Word Search II</t>
+  </si>
+  <si>
+    <t>This page has the list of probelems that ChatGPT could not solve.</t>
+  </si>
+  <si>
+    <t>Maybe these can be a measure for AGI</t>
   </si>
 </sst>
 </file>
@@ -435,6 +493,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA57C972-DDB5-4ED6-A55D-D7615711ABFB}" name="Table1" displayName="Table1" ref="A1:B2" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{BA57C972-DDB5-4ED6-A55D-D7615711ABFB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{03B1E253-EF8F-4B0D-A4A3-454DCD926646}" name="Problem Name"/>
+    <tableColumn id="2" xr3:uid="{1DFD506F-D572-423A-8D49-84675BF624D8}" name="Observation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,11 +771,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="19" ySplit="3" topLeftCell="T11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="19" ySplit="3" topLeftCell="T19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -2297,8 +2366,12 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="5">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="11"/>
@@ -2317,8 +2390,12 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="5">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="11"/>
@@ -2337,8 +2414,12 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="1:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="5">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="11"/>
@@ -2357,8 +2438,12 @@
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="1:18" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="5">
+        <v>30</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="11"/>
@@ -2377,8 +2462,12 @@
       <c r="R33" s="8"/>
     </row>
     <row r="34" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="5">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="11"/>
@@ -2397,8 +2486,12 @@
       <c r="R34" s="8"/>
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="5">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="11"/>
@@ -2417,8 +2510,12 @@
       <c r="R35" s="8"/>
     </row>
     <row r="36" spans="1:18" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="5">
+        <v>33</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="11"/>
@@ -2437,8 +2534,12 @@
       <c r="R36" s="8"/>
     </row>
     <row r="37" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="5">
+        <v>34</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="11"/>
@@ -2457,8 +2558,12 @@
       <c r="R37" s="8"/>
     </row>
     <row r="38" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="5">
+        <v>35</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="11"/>
@@ -2477,8 +2582,12 @@
       <c r="R38" s="8"/>
     </row>
     <row r="39" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="5">
+        <v>36</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="11"/>
@@ -2497,8 +2606,12 @@
       <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="5">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="11"/>
@@ -2517,8 +2630,12 @@
       <c r="R40" s="8"/>
     </row>
     <row r="41" spans="1:18" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="5">
+        <v>38</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="11"/>
@@ -2537,8 +2654,12 @@
       <c r="R41" s="8"/>
     </row>
     <row r="42" spans="1:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="5">
+        <v>39</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="11"/>
@@ -2557,8 +2678,12 @@
       <c r="R42" s="8"/>
     </row>
     <row r="43" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="5">
+        <v>40</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="11"/>
@@ -4193,4 +4318,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CDC6C4-838E-4E9E-B459-8069345A8D14}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added standard deviation and average statistics
</commit_message>
<xml_diff>
--- a/RQ1/RQ1.xlsx
+++ b/RQ1/RQ1.xlsx
@@ -8,27 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Documents\MastersDegree\CSI5370-SoftwareVerificationAndTesting\GithubRepos\csi5370project\RQ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B29E29-799E-40B4-8C08-6D0E17BCC3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2FC048-29BD-49FC-BC93-F6D6AE826AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-2535" windowWidth="29010" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34815" yWindow="-2535" windowWidth="34920" windowHeight="31785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main Data" sheetId="1" r:id="rId1"/>
-    <sheet name="ChatGPT" sheetId="2" r:id="rId2"/>
-    <sheet name="Analysis List" sheetId="3" r:id="rId3"/>
+    <sheet name="Main Data " sheetId="1" r:id="rId1"/>
+    <sheet name="Data (Hard)" sheetId="5" r:id="rId2"/>
+    <sheet name="Data (Medium)" sheetId="6" r:id="rId3"/>
+    <sheet name="ChatGPT" sheetId="2" r:id="rId4"/>
+    <sheet name="Analysis" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="144">
   <si>
     <t>SN</t>
   </si>
@@ -375,9 +388,6 @@
     <t>Array, Dynamic Programming, Prefix Sum</t>
   </si>
   <si>
-    <t>Anal</t>
-  </si>
-  <si>
     <t>Missed2</t>
   </si>
   <si>
@@ -391,13 +401,85 @@
   </si>
   <si>
     <t>Code Rate (out of 10)2</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Hard Problem</t>
+  </si>
+  <si>
+    <t>Medium Problems</t>
+  </si>
+  <si>
+    <t>Hard Problem2</t>
+  </si>
+  <si>
+    <t>ChatGPT Generated Code</t>
+  </si>
+  <si>
+    <t>PYNGUIN generated code</t>
+  </si>
+  <si>
+    <t>Medium Problems2</t>
+  </si>
+  <si>
+    <t>Overall PYNGUIN</t>
+  </si>
+  <si>
+    <t>Overall ChatGPT</t>
+  </si>
+  <si>
+    <t>Average Overall Code Coverage</t>
+  </si>
+  <si>
+    <t>Average Overall Code Quality</t>
+  </si>
+  <si>
+    <t>Number of Medium Problems</t>
+  </si>
+  <si>
+    <t>Number of Hard Problems</t>
+  </si>
+  <si>
+    <t>Average number of reprompts for test generation</t>
+  </si>
+  <si>
+    <t>Overall Code Coverage Standard Deviation</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>Statement2</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>PYNGUIN</t>
+  </si>
+  <si>
+    <t>Statements</t>
+  </si>
+  <si>
+    <t>Statements2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average </t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,8 +542,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,8 +590,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -630,6 +737,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -637,7 +755,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -717,6 +835,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -724,7 +869,196 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="32">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1460,33 +1794,87 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AF901C33-093E-4B07-BABC-303F55083690}" name="Table3" displayName="Table3" ref="A1:R57" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="20" tableBorderDxfId="21" headerRowCellStyle="Input">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AF901C33-093E-4B07-BABC-303F55083690}" name="Table3" displayName="Table3" ref="A1:R57" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11" headerRowBorderDxfId="30" tableBorderDxfId="31" headerRowCellStyle="Input">
   <autoFilter ref="A1:R57" xr:uid="{AF901C33-093E-4B07-BABC-303F55083690}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{14BF2805-2983-41D3-A905-EA29BE3EF091}" name="SN" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5E68D981-4EB7-49E1-9979-E0CED09B0BE8}" name="Leetcode Programming Problem" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A635F120-7CAD-4543-BA7A-D41DE84A34F1}" name="Difficulty Level" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{220E8640-E0CD-430B-89BE-F773CB0B5DA8}" name="Tags" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{246C5572-D894-4AA0-B2C9-03984E81C3AB}" name="Number of Solution  Submissions" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{92440134-69A9-427B-A9B7-C6B1CB312B66}" name="Number of Test Submissions" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{9D5AA59C-9730-4564-A59A-A6E7B66ED478}" name="ChatGPT Test Code Statistics" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{437D2347-4094-4C68-A977-C1A3E6342486}" name="Missed" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{B8FA1119-EF81-4F5D-A282-56A2F470A1A1}" name="Branch" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{075D7672-9E25-4E8D-9441-C051C5E4802B}" name="Partial Branch" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{851D7F01-997E-411B-9A72-F24092C7BF66}" name="Overall Coverage" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{ED4B7691-23A7-4CB4-AD3E-1CB856395D22}" name="Code Rate (out of 10)" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{2248D69E-11E2-4924-A1F3-3DEC05A667EB}" name="PYNGUIN Test Code Statistics" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{3744F41C-DFBE-42AE-8CB6-2B3926A86E4D}" name="Missed2" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{B3F8F93B-EC7C-4128-BD72-4236932BED8D}" name="Branch2" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{E16E6A39-B9F0-4793-8E8C-10B2EBE968B6}" name="Partial Branch2" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{4C6D652A-1B4C-441D-BD17-1F80502B9AC1}" name="Overall Coverage2" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{C564AAD1-5C8A-4861-AF27-0A825EA29488}" name="Code Rate (out of 10)2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{14BF2805-2983-41D3-A905-EA29BE3EF091}" name="SN" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{5E68D981-4EB7-49E1-9979-E0CED09B0BE8}" name="Leetcode Programming Problem" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{A635F120-7CAD-4543-BA7A-D41DE84A34F1}" name="Difficulty Level" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{220E8640-E0CD-430B-89BE-F773CB0B5DA8}" name="Tags" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{246C5572-D894-4AA0-B2C9-03984E81C3AB}" name="Number of Solution  Submissions" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{92440134-69A9-427B-A9B7-C6B1CB312B66}" name="Number of Test Submissions" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9D5AA59C-9730-4564-A59A-A6E7B66ED478}" name="ChatGPT Test Code Statistics" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{437D2347-4094-4C68-A977-C1A3E6342486}" name="Missed" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{B8FA1119-EF81-4F5D-A282-56A2F470A1A1}" name="Branch" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{075D7672-9E25-4E8D-9441-C051C5E4802B}" name="Partial Branch" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{851D7F01-997E-411B-9A72-F24092C7BF66}" name="Overall Coverage" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{ED4B7691-23A7-4CB4-AD3E-1CB856395D22}" name="Code Rate (out of 10)" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{2248D69E-11E2-4924-A1F3-3DEC05A667EB}" name="PYNGUIN Test Code Statistics" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{3744F41C-DFBE-42AE-8CB6-2B3926A86E4D}" name="Missed2" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{B3F8F93B-EC7C-4128-BD72-4236932BED8D}" name="Branch2" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{E16E6A39-B9F0-4793-8E8C-10B2EBE968B6}" name="Partial Branch2" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{4C6D652A-1B4C-441D-BD17-1F80502B9AC1}" name="Overall Coverage2" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{C564AAD1-5C8A-4861-AF27-0A825EA29488}" name="Code Rate (out of 10)2" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6A304295-7058-4D06-9C66-B87979418A34}" name="Table6" displayName="Table6" ref="A2:R27" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:R27" xr:uid="{6A304295-7058-4D06-9C66-B87979418A34}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{ECFED6CC-A20D-4320-97B8-B81083A4423A}" name="SN"/>
+    <tableColumn id="2" xr3:uid="{45B3B1F7-8916-4317-B3CF-EBC7A3815723}" name="Leetcode Programming Problem"/>
+    <tableColumn id="3" xr3:uid="{D3F21225-EC79-4610-9F21-08C43758A6EB}" name="Difficulty Level"/>
+    <tableColumn id="4" xr3:uid="{D17A717F-E17E-4CB2-95F2-B61445C0F889}" name="Tags"/>
+    <tableColumn id="5" xr3:uid="{C3C21B2E-5AB2-4D6E-BA86-8BF4399D5763}" name="Number of Solution  Submissions"/>
+    <tableColumn id="6" xr3:uid="{8A4165E0-4A85-4B89-986C-AA71201ED938}" name="Number of Test Submissions"/>
+    <tableColumn id="7" xr3:uid="{4B239765-FA90-4904-BF3E-546927817322}" name="Statements"/>
+    <tableColumn id="8" xr3:uid="{3A8E9E4F-52F0-4253-A053-0C67D5AB3129}" name="Missed"/>
+    <tableColumn id="9" xr3:uid="{33394F3F-9E2B-48C7-AC70-AB96BFD6B50A}" name="Branch"/>
+    <tableColumn id="10" xr3:uid="{75D49666-E14E-45A5-90D6-3859F23E5C8A}" name="Partial Branch"/>
+    <tableColumn id="11" xr3:uid="{CDD8942C-6C3D-4EFF-A71C-AF15309421F6}" name="Overall Coverage"/>
+    <tableColumn id="12" xr3:uid="{DB24E7F7-F199-43D0-B798-48CE3A6F0D3A}" name="Code Rate (out of 10)"/>
+    <tableColumn id="13" xr3:uid="{DBDBDBEC-A3AD-4E8D-9346-7C3C760AA8F2}" name="Statements2"/>
+    <tableColumn id="14" xr3:uid="{78161AB3-BD5C-4B18-8AD2-9F74E7780D02}" name="Missed2"/>
+    <tableColumn id="15" xr3:uid="{5E0F0963-0EDD-4152-92A5-734C4FA82BE4}" name="Branch2"/>
+    <tableColumn id="16" xr3:uid="{EEF02200-69DE-4689-ADD6-DAF20EA881E6}" name="Partial Branch2"/>
+    <tableColumn id="17" xr3:uid="{A2F6F09A-36C4-4B88-95A5-E177F09BA1E0}" name="Overall Coverage2"/>
+    <tableColumn id="18" xr3:uid="{D10F06A6-525E-4946-96FD-3B4EC78FA6D6}" name="Code Rate (out of 10)2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{401FC17F-D478-4B88-B9AE-7DBF04DBA35A}" name="Table7" displayName="Table7" ref="A2:R27" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:R27" xr:uid="{401FC17F-D478-4B88-B9AE-7DBF04DBA35A}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{F501BBE2-0AC9-42EC-ABDC-05ED4AC6DF75}" name="SN"/>
+    <tableColumn id="2" xr3:uid="{C6EBE987-6357-49E9-A567-18B8ADAEC2AC}" name="Leetcode Programming Problem"/>
+    <tableColumn id="3" xr3:uid="{9406AEE9-6204-463C-A1E6-687CE9FC04C6}" name="Difficulty Level"/>
+    <tableColumn id="4" xr3:uid="{D2F2A8AB-CCE6-48CF-8A18-0670AEBBA130}" name="Tags"/>
+    <tableColumn id="5" xr3:uid="{851A5B26-2EDC-4AF3-8E4D-3068AE0F120A}" name="Number of Solution  Submissions"/>
+    <tableColumn id="6" xr3:uid="{3D2A0BDA-B358-49BD-8793-3D827BD84BA8}" name="Number of Test Submissions"/>
+    <tableColumn id="7" xr3:uid="{D80D60DD-1E37-4AB7-954B-3E5F4715A034}" name="Statement"/>
+    <tableColumn id="8" xr3:uid="{B2468672-2586-4FFB-B63C-2D182B782CE5}" name="Missed"/>
+    <tableColumn id="9" xr3:uid="{0D33720A-48AC-43BD-B5D5-C1A7D69B8B79}" name="Branch"/>
+    <tableColumn id="10" xr3:uid="{5CBC48ED-8A2F-49A2-992B-5924A1CB00E3}" name="Partial Branch"/>
+    <tableColumn id="11" xr3:uid="{BC04AD6B-4F5D-444A-A5FD-E8FA2AB1F468}" name="Overall Coverage"/>
+    <tableColumn id="12" xr3:uid="{0A97C66C-6897-44DE-B9D0-0D090474A7C3}" name="Code Rate (out of 10)"/>
+    <tableColumn id="13" xr3:uid="{1066DDD4-7047-4811-BFDA-85838173C580}" name="Statement2"/>
+    <tableColumn id="14" xr3:uid="{035239A7-3575-4BD1-8A08-EC05B0377E97}" name="Missed2"/>
+    <tableColumn id="15" xr3:uid="{ED957F9E-FAE3-489F-9616-A1DA3EC7D831}" name="Branch2"/>
+    <tableColumn id="16" xr3:uid="{48886ECB-D5DC-4348-AAB7-9CD7E636AFFF}" name="Partial Branch2"/>
+    <tableColumn id="17" xr3:uid="{D93A7BAE-0ED3-44F2-B1A8-44833B478F34}" name="Overall Coverage2"/>
+    <tableColumn id="18" xr3:uid="{7EFF2689-F41D-4922-87E8-1F0E2F4497FC}" name="Code Rate (out of 10)2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA57C972-DDB5-4ED6-A55D-D7615711ABFB}" name="Table1" displayName="Table1" ref="A1:B2" insertRowShift="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{BA57C972-DDB5-4ED6-A55D-D7615711ABFB}"/>
   <tableColumns count="2">
@@ -1494,6 +1882,28 @@
     <tableColumn id="2" xr3:uid="{1DFD506F-D572-423A-8D49-84675BF624D8}" name="Observation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7DC8C4C4-6BC6-4EB4-8DFD-93DFA48503BE}" name="Table5" displayName="Table5" ref="A2:G21" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A2:G21" xr:uid="{7DC8C4C4-6BC6-4EB4-8DFD-93DFA48503BE}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CE7E8AC1-2ECD-4D2C-9AD8-A8F48438B055}" name="Statistics" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3F58C3D0-56C0-42CF-ABF5-0EF8978B404D}" name="Hard Problem" dataDxfId="2">
+      <calculatedColumnFormula>AVERAGE('Main Data '!K5:K53)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{2A207C60-57DC-43B9-B963-CB78F11C81BB}" name="Medium Problems" dataDxfId="4">
+      <calculatedColumnFormula>AVERAGE('Main Data '!K4:K51)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B1FA7B39-4D44-4B45-8414-BC25AFE80B76}" name="Overall ChatGPT" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{7E2E48CA-24C5-4192-AFB7-F7D05EC58863}" name="Hard Problem2" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C597DDFA-F185-4CB2-9C71-BACC88AFAFDF}" name="Medium Problems2" dataDxfId="3">
+      <calculatedColumnFormula>AVERAGE('Main Data '!Q4:Q51)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{7635FA6F-64D5-4702-B1DA-90A20653FFE6}" name="Overall PYNGUIN" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1760,13 +2170,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:W123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="19" ySplit="3" topLeftCell="T40" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="19" ySplit="3" topLeftCell="T30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomRight" activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1830,19 +2240,19 @@
         <v>7</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -3885,7 +4295,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>108</v>
@@ -4437,7 +4847,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13">
         <v>46</v>
       </c>
@@ -4493,7 +4903,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="13">
         <v>47</v>
       </c>
@@ -4549,7 +4959,7 @@
         <v>5.67</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13">
         <v>48</v>
       </c>
@@ -4605,7 +5015,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13">
         <v>49</v>
       </c>
@@ -4661,7 +5071,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="139.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="139.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13">
         <v>50</v>
       </c>
@@ -4717,7 +5127,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4737,47 +5147,97 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="14"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A55" s="13"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="14"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B55" s="38"/>
+      <c r="C55" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38">
+        <f>AVERAGE(E4:E53)</f>
+        <v>1.24</v>
+      </c>
+      <c r="F55" s="38">
+        <f>AVERAGE(F4:F53)</f>
+        <v>2.86</v>
+      </c>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38">
+        <f>AVERAGE(K4:K53)</f>
+        <v>94.58</v>
+      </c>
+      <c r="L55" s="38">
+        <f>AVERAGE(L4:L53)</f>
+        <v>3.7976000000000005</v>
+      </c>
+      <c r="M55" s="38"/>
+      <c r="N55" s="38"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38">
+        <f>AVERAGE(Q4:Q53)</f>
+        <v>100</v>
+      </c>
+      <c r="R55" s="38">
+        <f>AVERAGE(R4:R53)</f>
+        <v>4.6560000000000006</v>
+      </c>
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="39"/>
+      <c r="V55" s="39"/>
+      <c r="W55" s="39"/>
+    </row>
+    <row r="56" spans="1:23" ht="63" x14ac:dyDescent="0.5">
       <c r="A56" s="13"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="14"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B56" s="38"/>
+      <c r="C56" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38">
+        <f>STDEV(E4:E53)</f>
+        <v>0.43141911058690008</v>
+      </c>
+      <c r="F56" s="38">
+        <f>STDEV(F4:F53)</f>
+        <v>1.7613770123377437</v>
+      </c>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38">
+        <f>STDEV(K4:K53)</f>
+        <v>9.4460660205879439</v>
+      </c>
+      <c r="L56" s="38">
+        <f>STDEV(L4:L53)</f>
+        <v>2.520085486078369</v>
+      </c>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="38"/>
+      <c r="P56" s="38"/>
+      <c r="Q56" s="38">
+        <f>STDEV(Q4:Q53)</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="38">
+        <f>STDEV(R4:R53)</f>
+        <v>2.2805522066698956</v>
+      </c>
+      <c r="S56" s="39"/>
+      <c r="T56" s="39"/>
+      <c r="U56" s="39"/>
+      <c r="V56" s="39"/>
+      <c r="W56" s="39"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="15"/>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
@@ -4797,7 +5257,7 @@
       <c r="Q57" s="16"/>
       <c r="R57" s="19"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4817,7 +5277,7 @@
       <c r="Q58" s="3"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4837,7 +5297,7 @@
       <c r="Q59" s="3"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4857,7 +5317,7 @@
       <c r="Q60" s="3"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4877,7 +5337,7 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4897,7 +5357,7 @@
       <c r="Q62" s="3"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4917,7 +5377,7 @@
       <c r="Q63" s="3"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6128,11 +6588,3156 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7162F10A-21E6-4154-A952-1239DEC1383A}">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+    </row>
+    <row r="2" spans="1:18" s="36" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>36</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>1.2</v>
+      </c>
+      <c r="M4">
+        <v>19</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>59</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>45</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>7.11</v>
+      </c>
+      <c r="M6">
+        <v>53</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>17</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="M8">
+        <v>42</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>42</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>12</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>26</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>6.54</v>
+      </c>
+      <c r="M10">
+        <v>13</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>91</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>76</v>
+      </c>
+      <c r="L12">
+        <v>4.07</v>
+      </c>
+      <c r="M12">
+        <v>21</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+      <c r="R12">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>33</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>89</v>
+      </c>
+      <c r="L13">
+        <v>7.5</v>
+      </c>
+      <c r="M13">
+        <v>41</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>100</v>
+      </c>
+      <c r="R13">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>4.76</v>
+      </c>
+      <c r="M14">
+        <v>70</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>100</v>
+      </c>
+      <c r="R14">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>0.65</v>
+      </c>
+      <c r="M15">
+        <v>33</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>100</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>100</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>18</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="M17">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>100</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>96</v>
+      </c>
+      <c r="L18">
+        <v>3.1</v>
+      </c>
+      <c r="M18">
+        <v>103</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>100</v>
+      </c>
+      <c r="R18">
+        <v>8.1199999999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <v>3.85</v>
+      </c>
+      <c r="M19">
+        <v>14</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>100</v>
+      </c>
+      <c r="R19">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>26</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="M20">
+        <v>24</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>100</v>
+      </c>
+      <c r="R20">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>95</v>
+      </c>
+      <c r="L21">
+        <v>5.56</v>
+      </c>
+      <c r="M21">
+        <v>27</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>100</v>
+      </c>
+      <c r="R21">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>32</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>75</v>
+      </c>
+      <c r="L22">
+        <v>6.33</v>
+      </c>
+      <c r="M22">
+        <v>41</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>100</v>
+      </c>
+      <c r="R22">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23">
+        <v>12</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>71</v>
+      </c>
+      <c r="L23">
+        <v>7.57</v>
+      </c>
+      <c r="M23">
+        <v>17</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>26</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24">
+        <v>5.77</v>
+      </c>
+      <c r="M24">
+        <v>15</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>93</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>34</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>17</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>94</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>35</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>100</v>
+      </c>
+      <c r="R26">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>64</v>
+      </c>
+      <c r="L27">
+        <v>0.91</v>
+      </c>
+      <c r="M27">
+        <v>17</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(Table6[Number of Solution  Submissions])</f>
+        <v>1.28</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(Table6[Number of Test Submissions])</f>
+        <v>3.32</v>
+      </c>
+      <c r="K29">
+        <f>AVERAGE(Table6[Overall Coverage])</f>
+        <v>93.76</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(Table6[Code Rate (out of 10)])</f>
+        <v>3.1328000000000005</v>
+      </c>
+      <c r="Q29">
+        <f>AVERAGE(Table6[Overall Coverage2])</f>
+        <v>100</v>
+      </c>
+      <c r="R29">
+        <f>AVERAGE(Table6[Code Rate (out of 10)2])</f>
+        <v>4.3260000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30">
+        <f>STDEV(Table6[Number of Solution  Submissions])</f>
+        <v>0.45825756949558394</v>
+      </c>
+      <c r="F30">
+        <f>STDEV(Table6[Number of Test Submissions])</f>
+        <v>1.7009801096230763</v>
+      </c>
+      <c r="K30">
+        <f>STDEV(Table6[Overall Coverage])</f>
+        <v>10.591978096654085</v>
+      </c>
+      <c r="L30">
+        <f>STDEV(Table6[Code Rate (out of 10)])</f>
+        <v>2.7669726537619894</v>
+      </c>
+      <c r="Q30">
+        <f>STDEV(Table6[Overall Coverage2])</f>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f>STDEV(Table6[Code Rate (out of 10)2])</f>
+        <v>2.2999402166143352</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B088F6BB-6430-4CD8-95EF-5A7AB565F0A4}">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+    </row>
+    <row r="2" spans="1:18" s="36" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>6.25</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>51</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>50</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>3.91</v>
+      </c>
+      <c r="M6">
+        <v>113</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>3.33</v>
+      </c>
+      <c r="M7">
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>8</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>98</v>
+      </c>
+      <c r="L8">
+        <v>7.91</v>
+      </c>
+      <c r="M8">
+        <v>65</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>95</v>
+      </c>
+      <c r="L9">
+        <v>6.15</v>
+      </c>
+      <c r="M9">
+        <v>39</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>25</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>22</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>5.45</v>
+      </c>
+      <c r="M11">
+        <v>14</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>4.21</v>
+      </c>
+      <c r="M12">
+        <v>96</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+      <c r="R12">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>74</v>
+      </c>
+      <c r="L13">
+        <v>6.54</v>
+      </c>
+      <c r="M13">
+        <v>26</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>6</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>100</v>
+      </c>
+      <c r="R13">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>5.5</v>
+      </c>
+      <c r="M14">
+        <v>25</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>100</v>
+      </c>
+      <c r="R14">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>27</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>90</v>
+      </c>
+      <c r="L15">
+        <v>6.92</v>
+      </c>
+      <c r="M15">
+        <v>21</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>100</v>
+      </c>
+      <c r="R15">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>29</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>76</v>
+      </c>
+      <c r="L16">
+        <v>7.04</v>
+      </c>
+      <c r="M16">
+        <v>31</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>8</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>100</v>
+      </c>
+      <c r="R16">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>88</v>
+      </c>
+      <c r="L17">
+        <v>6.36</v>
+      </c>
+      <c r="M17">
+        <v>24</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>100</v>
+      </c>
+      <c r="R17">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>37</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="M18">
+        <v>52</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>100</v>
+      </c>
+      <c r="R18">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>33</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <v>5.31</v>
+      </c>
+      <c r="M19">
+        <v>19</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>100</v>
+      </c>
+      <c r="R19">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>2.65</v>
+      </c>
+      <c r="M20">
+        <v>33</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>100</v>
+      </c>
+      <c r="R20">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>38</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>3.42</v>
+      </c>
+      <c r="M21">
+        <v>15</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>100</v>
+      </c>
+      <c r="R21">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>0.5</v>
+      </c>
+      <c r="M22">
+        <v>46</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>100</v>
+      </c>
+      <c r="R22">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>16</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23">
+        <v>3.75</v>
+      </c>
+      <c r="M23">
+        <v>22</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24">
+        <v>4.67</v>
+      </c>
+      <c r="M24">
+        <v>74</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <v>7.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>100</v>
+      </c>
+      <c r="L25">
+        <v>4.5</v>
+      </c>
+      <c r="M25">
+        <v>39</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>83</v>
+      </c>
+      <c r="L26">
+        <v>3.33</v>
+      </c>
+      <c r="M26">
+        <v>31</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>100</v>
+      </c>
+      <c r="R26">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>21</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>81</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>14</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(Table7[Number of Solution  Submissions])</f>
+        <v>1.2</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(Table7[Number of Test Submissions])</f>
+        <v>2.4</v>
+      </c>
+      <c r="K29">
+        <f>AVERAGE(Table7[Overall Coverage])</f>
+        <v>95.4</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(Table7[Code Rate (out of 10)])</f>
+        <v>4.4624000000000006</v>
+      </c>
+      <c r="Q29">
+        <f>AVERAGE(Table7[Overall Coverage2])</f>
+        <v>100</v>
+      </c>
+      <c r="R29">
+        <f>AVERAGE(Table7[Code Rate (out of 10)2])</f>
+        <v>4.9860000000000015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30">
+        <f>STDEV(Table7[Number of Solution  Submissions])</f>
+        <v>0.40824829046386302</v>
+      </c>
+      <c r="F30">
+        <f>STDEV(Table7[Number of Test Submissions])</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="K30">
+        <f>STDEV(Table7[Overall Coverage])</f>
+        <v>8.2815054992032273</v>
+      </c>
+      <c r="L30">
+        <f>STDEV(Table7[Code Rate (out of 10)])</f>
+        <v>2.0950880649748331</v>
+      </c>
+      <c r="Q30">
+        <f>STDEV(Table7[Overall Coverage2])</f>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f>STDEV(Table7[Code Rate (out of 10)2])</f>
+        <v>2.2587478094436855</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CDC6C4-838E-4E9E-B459-8069345A8D14}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6171,20 +9776,275 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC562970-E38E-4F98-9878-3EE8686FAFB4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>115</v>
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>